<commit_message>
Começando a preencher a planilha
</commit_message>
<xml_diff>
--- a/compute_diffusivities/dados_isotermas.xlsx
+++ b/compute_diffusivities/dados_isotermas.xlsx
@@ -1,32 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="dados" sheetId="1" r:id="rId1"/>
-    <sheet name="calculos" sheetId="2" r:id="rId2"/>
+    <sheet name="CH4" sheetId="1" r:id="rId1"/>
+    <sheet name="H2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
-    <t>P (bar)</t>
+    <t>C [mol/g]</t>
   </si>
   <si>
-    <t>CH4</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>P (MPa)</t>
+    <t>P [MPa]</t>
   </si>
 </sst>
 </file>
@@ -62,8 +56,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -124,7 +119,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -159,7 +154,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -368,7 +363,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.26</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.41E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.79</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3.15E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1.26</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.9500000000000004E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.74</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.4200000000000003E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -376,79 +430,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>calculos!A2*10</f>
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.74</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.2000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>calculos!A3*10</f>
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.32</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3.8000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>calculos!A4*10</f>
-        <v>12.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.78</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7.2999999999999996E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>calculos!A5*10</f>
-        <v>17.399999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1.74</v>
+        <v>3.31</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8.9999999999999998E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>